<commit_message>
feat: refatoração inicial para processamento baseado em máquina
Comentário temporário: trabalhando no novo arquivo de processamento para relatório baseado em máquina.
</commit_message>
<xml_diff>
--- a/dados/CAV OUROESTE.xlsx
+++ b/dados/CAV OUROESTE.xlsx
@@ -97,10 +97,10 @@
     <t>485699</t>
   </si>
   <si>
-    <t>09/07/2025 00:00</t>
-  </si>
-  <si>
-    <t>09/07/2025 23:59</t>
+    <t>14/07/2025 00:00</t>
+  </si>
+  <si>
+    <t>14/07/2025 23:59</t>
   </si>
   <si>
     <t>6126</t>
@@ -682,46 +682,46 @@
         <v>29</v>
       </c>
       <c r="I2">
-        <v>21.25</v>
+        <v>11.75</v>
       </c>
       <c r="J2">
-        <v>8559.85</v>
+        <v>8640.9</v>
       </c>
       <c r="K2">
-        <v>65.76297861111112</v>
+        <v>43.144257222222215</v>
       </c>
       <c r="L2">
-        <v>251.80620111111108</v>
+        <v>128.25583749999998</v>
       </c>
       <c r="M2">
-        <v>4.147515555555556</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>6.848165432749844</v>
+        <v>6.485298931423896</v>
       </c>
       <c r="O2">
-        <v>19.31734056076518</v>
+        <v>20.791240116174354</v>
       </c>
       <c r="P2">
-        <v>31.548538282078475</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>321.71669444444456</v>
+        <v>171.40009583333335</v>
       </c>
       <c r="R2">
-        <v>1061.507607791788</v>
+        <v>565.5364140101952</v>
       </c>
       <c r="S2">
-        <v>0.528</v>
+        <v>0.588</v>
       </c>
       <c r="T2">
-        <v>14.134371329862235</v>
+        <v>13.403557774303266</v>
       </c>
       <c r="U2">
-        <v>46.636506457683396</v>
+        <v>44.22517946564514</v>
       </c>
       <c r="V2">
-        <v>0.2766590521299549</v>
+        <v>0.2735561070501127</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -779,7 +779,7 @@
         <v>29</v>
       </c>
       <c r="J4">
-        <v>8252.2</v>
+        <v>8254.45</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -866,46 +866,46 @@
         <v>29</v>
       </c>
       <c r="I7">
-        <v>18.950000000000728</v>
+        <v>12.949999999998909</v>
       </c>
       <c r="J7">
-        <v>8815.15</v>
+        <v>8891</v>
       </c>
       <c r="K7">
-        <v>52.185173333333346</v>
+        <v>37.514920277777776</v>
       </c>
       <c r="L7">
-        <v>200.15389666666672</v>
+        <v>128.04666194444442</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>1.7534527777777777</v>
       </c>
       <c r="N7">
-        <v>6.011568099294014</v>
+        <v>6.396066852968526</v>
       </c>
       <c r="O7">
-        <v>18.574200652755643</v>
+        <v>15.766277080704343</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>20.347662779397474</v>
       </c>
       <c r="Q7">
-        <v>252.33906944444445</v>
+        <v>167.31503611111114</v>
       </c>
       <c r="R7">
-        <v>832.5954064054121</v>
+        <v>552.0577166087103</v>
       </c>
       <c r="S7">
-        <v>0.648</v>
+        <v>0.6679999999999999</v>
       </c>
       <c r="T7">
-        <v>12.979247414469814</v>
+        <v>11.916687393131028</v>
       </c>
       <c r="U7">
-        <v>42.82516298280186</v>
+        <v>39.31923504724892</v>
       </c>
       <c r="V7">
-        <v>0.28439576969728103</v>
+        <v>0.2869238584198225</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -934,46 +934,46 @@
         <v>29</v>
       </c>
       <c r="I8">
-        <v>18.550000000000182</v>
+        <v>19.849999999999454</v>
       </c>
       <c r="J8">
-        <v>6852</v>
+        <v>6938.6</v>
       </c>
       <c r="K8">
-        <v>43.01744305555556</v>
+        <v>49.53759805555555</v>
       </c>
       <c r="L8">
-        <v>169.49053305555552</v>
+        <v>179.05847416666666</v>
       </c>
       <c r="M8">
-        <v>0.17496111111111112</v>
+        <v>15.846829722222223</v>
       </c>
       <c r="N8">
-        <v>4.72302430090951</v>
+        <v>4.696134463129835</v>
       </c>
       <c r="O8">
-        <v>17.661678476307372</v>
+        <v>18.0240630281001</v>
       </c>
       <c r="P8">
-        <v>22.783</v>
+        <v>31.132404060248856</v>
       </c>
       <c r="Q8">
-        <v>212.6829369444444</v>
+        <v>244.44290305555555</v>
       </c>
       <c r="R8">
-        <v>701.7495812702218</v>
+        <v>806.5419225827291</v>
       </c>
       <c r="S8">
-        <v>0.44799999999999995</v>
+        <v>0.348</v>
       </c>
       <c r="T8">
-        <v>11.400734095962987</v>
+        <v>11.673197163243074</v>
       </c>
       <c r="U8">
-        <v>37.616841731431386</v>
+        <v>38.51583647977524</v>
       </c>
       <c r="V8">
-        <v>0.2520571106420659</v>
+        <v>0.26152155813881867</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1002,46 +1002,46 @@
         <v>29</v>
       </c>
       <c r="I9">
-        <v>17.350000000000364</v>
+        <v>20.25</v>
       </c>
       <c r="J9">
-        <v>7667.3</v>
+        <v>7751.15</v>
       </c>
       <c r="K9">
-        <v>37.183995555555555</v>
+        <v>44.40174249999997</v>
       </c>
       <c r="L9">
-        <v>159.19253916666668</v>
+        <v>191.86119472222222</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>16.12675638888889</v>
       </c>
       <c r="N9">
-        <v>4.661396565709286</v>
+        <v>4.4769097016299195</v>
       </c>
       <c r="O9">
-        <v>15.414636364125407</v>
+        <v>18.142762121514572</v>
       </c>
       <c r="P9">
-        <v>0</v>
+        <v>32.5412461038233</v>
       </c>
       <c r="Q9">
-        <v>196.3765341666667</v>
+        <v>252.38969444444444</v>
       </c>
       <c r="R9">
-        <v>647.9464342677984</v>
+        <v>832.7624441239154</v>
       </c>
       <c r="S9">
-        <v>0.6679999999999999</v>
+        <v>0.588</v>
       </c>
       <c r="T9">
-        <v>10.762086825689417</v>
+        <v>12.065113772216096</v>
       </c>
       <c r="U9">
-        <v>35.50961836442045</v>
+        <v>39.8089694418779</v>
       </c>
       <c r="V9">
-        <v>0.2499447194553732</v>
+        <v>0.2624503201294111</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1070,46 +1070,46 @@
         <v>29</v>
       </c>
       <c r="I10">
-        <v>17.5</v>
+        <v>12.199999999998909</v>
       </c>
       <c r="J10">
-        <v>9263.2</v>
+        <v>9340.15</v>
       </c>
       <c r="K10">
-        <v>41.343059444444435</v>
+        <v>22.452311388888887</v>
       </c>
       <c r="L10">
-        <v>172.31346972222224</v>
+        <v>125.8994411111111</v>
       </c>
       <c r="M10">
-        <v>0.5736955555555556</v>
+        <v>6.5919847222222225</v>
       </c>
       <c r="N10">
-        <v>4.80409220334124</v>
+        <v>4.366760849644152</v>
       </c>
       <c r="O10">
-        <v>19.046358675762637</v>
+        <v>15.558125661493689</v>
       </c>
       <c r="P10">
-        <v>29.239000000000004</v>
+        <v>29.57345411352838</v>
       </c>
       <c r="Q10">
-        <v>214.23022638888898</v>
+        <v>154.94373611111112</v>
       </c>
       <c r="R10">
-        <v>706.854879021618</v>
+        <v>511.2384824966854</v>
       </c>
       <c r="S10">
-        <v>0.648</v>
+        <v>0.72</v>
       </c>
       <c r="T10">
-        <v>12.155247076729726</v>
+        <v>11.556279717622635</v>
       </c>
       <c r="U10">
-        <v>40.10636522552491</v>
+        <v>38.13006614160862</v>
       </c>
       <c r="V10">
-        <v>0.2684337143311384</v>
+        <v>0.25883073164200204</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -1138,46 +1138,46 @@
         <v>29</v>
       </c>
       <c r="I11">
-        <v>20.450000000000728</v>
+        <v>10.799999999999272</v>
       </c>
       <c r="J11">
-        <v>8651.45</v>
+        <v>8720.1</v>
       </c>
       <c r="K11">
-        <v>64.13018027777777</v>
+        <v>41.85617972222224</v>
       </c>
       <c r="L11">
-        <v>225.74760583333332</v>
+        <v>85.46789499999998</v>
       </c>
       <c r="M11">
-        <v>1.273263888888889</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>6.715942025972792</v>
+        <v>6.290916353399304</v>
       </c>
       <c r="O11">
-        <v>19.734337067002077</v>
+        <v>18.877239733002856</v>
       </c>
       <c r="P11">
-        <v>28.679822166562303</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>291.15104472222225</v>
+        <v>127.32407527777781</v>
       </c>
       <c r="R11">
-        <v>960.6559259315518</v>
+        <v>420.1071218756871</v>
       </c>
       <c r="S11">
-        <v>0.54</v>
+        <v>0.728</v>
       </c>
       <c r="T11">
-        <v>13.90964613848557</v>
+        <v>11.416189176630477</v>
       </c>
       <c r="U11">
-        <v>45.89502333160338</v>
+        <v>37.667835932201434</v>
       </c>
       <c r="V11">
-        <v>0.29067039688021745</v>
+        <v>0.29207950126470683</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -1206,46 +1206,46 @@
         <v>29</v>
       </c>
       <c r="I12">
-        <v>5.350000000000136</v>
+        <v>20.34999999999991</v>
       </c>
       <c r="J12">
-        <v>1209.8</v>
+        <v>1297.7</v>
       </c>
       <c r="K12">
-        <v>23.663080555555556</v>
+        <v>97.21722555555556</v>
       </c>
       <c r="L12">
-        <v>54.338640555555564</v>
+        <v>243.83604527777783</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>0.15145416666666667</v>
       </c>
       <c r="N12">
-        <v>9.949527979540836</v>
+        <v>10.36700631747301</v>
       </c>
       <c r="O12">
-        <v>17.87273413731671</v>
+        <v>20.515931265847936</v>
       </c>
       <c r="P12">
-        <v>0</v>
+        <v>17.08</v>
       </c>
       <c r="Q12">
-        <v>78.0017225</v>
+        <v>341.2047233333334</v>
       </c>
       <c r="R12">
-        <v>257.3675015454072</v>
+        <v>1125.8085635197597</v>
       </c>
       <c r="S12">
-        <v>0.9520000000000001</v>
+        <v>0.54</v>
       </c>
       <c r="T12">
-        <v>14.394911322524594</v>
+        <v>16.040236089620798</v>
       </c>
       <c r="U12">
-        <v>47.496160896265444</v>
+        <v>52.92492722303892</v>
       </c>
       <c r="V12">
-        <v>0.3368312176392695</v>
+        <v>0.3470115614232021</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -1274,46 +1274,46 @@
         <v>29</v>
       </c>
       <c r="I13">
-        <v>5.150000000000091</v>
+        <v>12.549999999999955</v>
       </c>
       <c r="J13">
-        <v>1204.2</v>
+        <v>1285</v>
       </c>
       <c r="K13">
-        <v>19.04589361111111</v>
+        <v>34.99618527777777</v>
       </c>
       <c r="L13">
-        <v>40.087628611111114</v>
+        <v>128.09865416666668</v>
       </c>
       <c r="M13">
-        <v>0.15976666666666667</v>
+        <v>1.5333794444444444</v>
       </c>
       <c r="N13">
-        <v>6.9562377112368905</v>
+        <v>6.720012158897594</v>
       </c>
       <c r="O13">
-        <v>16.596863687587682</v>
+        <v>16.765228576102366</v>
       </c>
       <c r="P13">
-        <v>21.895</v>
+        <v>30.068526488257785</v>
       </c>
       <c r="Q13">
-        <v>59.29328833333332</v>
+        <v>164.62822027777779</v>
       </c>
       <c r="R13">
-        <v>195.63882678054244</v>
+        <v>543.192539584733</v>
       </c>
       <c r="S13">
-        <v>0.9279999999999999</v>
+        <v>0.536</v>
       </c>
       <c r="T13">
-        <v>11.48901356238698</v>
+        <v>12.762036086625125</v>
       </c>
       <c r="U13">
-        <v>37.90812075685682</v>
+        <v>42.10847192825818</v>
       </c>
       <c r="V13">
-        <v>0.3316065579234585</v>
+        <v>0.31177736835312886</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1487,46 +1487,46 @@
         <v>29</v>
       </c>
       <c r="I19">
-        <v>14.650000000000091</v>
+        <v>14.600000000000136</v>
       </c>
       <c r="J19">
-        <v>1291.3</v>
+        <v>1383.45</v>
       </c>
       <c r="K19">
-        <v>78.68424583333332</v>
+        <v>81.35426861111114</v>
       </c>
       <c r="L19">
-        <v>133.64608527777781</v>
+        <v>135.13235194444445</v>
       </c>
       <c r="M19">
-        <v>0</v>
+        <v>1.0984266666666667</v>
       </c>
       <c r="N19">
-        <v>10.26967149863523</v>
+        <v>10.375846784363175</v>
       </c>
       <c r="O19">
-        <v>19.091449199282607</v>
+        <v>18.8633921143646</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>24.31918411330049</v>
       </c>
       <c r="Q19">
-        <v>212.3303286111111</v>
+        <v>217.58504666666656</v>
       </c>
       <c r="R19">
-        <v>700.5861463758952</v>
+        <v>717.9241437167084</v>
       </c>
       <c r="S19">
-        <v>0.78</v>
+        <v>0.532</v>
       </c>
       <c r="T19">
-        <v>14.481302228662894</v>
+        <v>14.457798059958218</v>
       </c>
       <c r="U19">
-        <v>47.7812085972192</v>
+        <v>47.70365634604392</v>
       </c>
       <c r="V19">
-        <v>0.3888274939083317</v>
+        <v>0.39373101772039976</v>
       </c>
     </row>
   </sheetData>

</xml_diff>